<commit_message>
Corrected nand2x delay Value in fanout8
</commit_message>
<xml_diff>
--- a/Assignment1/assets/Delay xlsx files/Nand_Delay - 2x.xlsx
+++ b/Assignment1/assets/Delay xlsx files/Nand_Delay - 2x.xlsx
@@ -610,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1281,7 +1281,7 @@
         <v>13</v>
       </c>
       <c r="F36" s="9">
-        <v>2.6023600000000002E-11</v>
+        <v>3.3030000000000001E-11</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
@@ -1299,7 +1299,7 @@
         <v>15</v>
       </c>
       <c r="F37" s="9">
-        <v>3.3030000000000001E-11</v>
+        <v>2.6023600000000002E-11</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">

</xml_diff>